<commit_message>
finished TGZ-D-320 added TGZ-S-400 3/9 - not finished yet
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/parameters.xlsx
+++ b/docs/Manual/source/CZ/tab/parameters.xlsx
@@ -5,18 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="TGZ-D-48-50_100" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="TGZ-S-48-50_100" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="TGZ-S-48-100_250" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="TGZ-S-48-100_300" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="TGZ-S-48-100_425" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="TGZ-S-230-5_15" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="TGZ-D-320-5_10" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="TGZ-D-320-5_15" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="TGZ-D-48-50_100" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="TGZ-S-48-50_100" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="TGZ-S-48-100_250" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="TGZ-S-48-100_300" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="TGZ-S-48-100_425" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="TGZ-S-230-5_15" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="TGZ-D-320-5_10" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="TGZ-D-320-5_15" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="TGZ-S-400-3_9" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="TGZ-S-400-7_15" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="TGZ-S-400-10_20" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="TGZ-S-400-14_30" sheetId="13" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="107">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -292,6 +296,63 @@
   </si>
   <si>
     <t xml:space="preserve">2 x 8pin WEIDMÜLLER  B2CF 3.50/08/180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 VAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,7 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pracovní spínací frekvence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 kHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 12pin WEIDMÜLLER BLZ 7.62HP/12/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 6pin WEIDMÜLLER  BLF 7.62HP/06/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCZXX3P49-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,9 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,6 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,4 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 kHz</t>
   </si>
 </sst>
 </file>
@@ -369,17 +430,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -394,8 +467,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -407,191 +586,191 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -606,8 +785,992 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -619,199 +1782,199 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -827,7 +1990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -839,191 +2002,191 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1039,7 +2202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1051,199 +2214,199 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1259,7 +2422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1271,199 +2434,199 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1479,7 +2642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1491,199 +2654,199 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1699,208 +2862,208 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1916,7 +3079,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1928,191 +3091,191 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2128,7 +3291,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2140,191 +3303,191 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pridany TGM a Ostatni kategorie rozpracovan TGMmini manual
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/parameters.xlsx
+++ b/docs/Manual/source/CZ/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,6 +23,8 @@
     <sheet name="TGZ-S-400-14_30" sheetId="13" state="visible" r:id="rId15"/>
     <sheet name="TGZ-D-560-30_50" sheetId="14" state="visible" r:id="rId16"/>
     <sheet name="TGS-320-10_15" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="TGS-560-25_50" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="TGS-560-50_100" sheetId="17" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="164">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -480,10 +482,52 @@
     <t xml:space="preserve">1 x 8pin PHOENIX PC 5/ 8-STCL1-7,62</t>
   </si>
   <si>
-    <t xml:space="preserve">Konektor pro digitální výstupy</t>
+    <t xml:space="preserve">Konektor pro kontrolní výstupy</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 4pin WEIDMÜLLER BCZ 3.81/04/180 SN BK BX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 x 400 VAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">560 VDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 5pin WEIDMÜLLER BCZ 3.81/05/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 7pin WAGO push-in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI konektor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Připojení externího termistoru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x 2pin WEIDMÜLLER LSF (push-in)</t>
   </si>
 </sst>
 </file>
@@ -712,7 +756,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,7 +968,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1170,7 +1214,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1416,7 +1460,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1662,7 +1706,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1908,7 +1952,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="1" sqref="A1:B30 C38"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2140,8 +2184,8 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="A1:B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2376,6 +2420,532 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2396,7 +2966,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2616,7 +3186,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2828,7 +3398,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3048,7 +3618,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3268,7 +3838,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3488,7 +4058,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3705,7 +4275,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3917,7 +4487,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="A1:B30"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
dokoncen TGMcontroller dokoncen TGZ+Motion TGMotion pridan do extra struktury (nespada pod TGM zalozku)
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/parameters.xlsx
+++ b/docs/Manual/source/CZ/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,6 +27,7 @@
     <sheet name="TGS-560-50_100" sheetId="17" state="visible" r:id="rId19"/>
     <sheet name="TGMmini" sheetId="18" state="visible" r:id="rId20"/>
     <sheet name="TGMcontroller" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="TGZpMotion" sheetId="20" state="visible" r:id="rId22"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="188">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -3066,7 +3067,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3074,7 +3075,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3464,6 +3465,167 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">

</xml_diff>

<commit_message>
testy se 3D modely three.js (neúspěšné) přidána sekce Společný HW - detailní popis IO atd
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/parameters.xlsx
+++ b/docs/Manual/source/CZ/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -31,6 +31,7 @@
     <sheet name="TGMmini" sheetId="21" state="visible" r:id="rId23"/>
     <sheet name="TGMcontroller" sheetId="22" state="visible" r:id="rId24"/>
     <sheet name="TGZpMotion" sheetId="23" state="visible" r:id="rId25"/>
+    <sheet name="commonHW_DI" sheetId="24" state="visible" r:id="rId26"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="262">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -729,6 +730,105 @@
   </si>
   <si>
     <t xml:space="preserve">Červená/zelená dioda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> č. vstupu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rozsah napětí log. 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rozsah napětí log. 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nominální vstupní napětí </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rozsah napájení DI/DO </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> spotřeba v log. 1 (17V) ±20% </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> spotřeba v log. 1 (24V) ±20% </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vlastní spotřeba v log.1 (28V) ±20% </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nominální vstupní odpor ±20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Přiřazeno k ose </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Max. vstupní frekvence - obdélník </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U&lt;sub&gt;log0&lt;/sub&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U&lt;sub&gt;log1&lt;/sub&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U&lt;sub&gt;nom&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VDD&lt;sub&gt;IO&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I&lt;sub&gt;in17&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I&lt;sub&gt;in24&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I&lt;sub&gt;in28&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RI&lt;sub&gt;inNom&lt;/sub&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Osa č. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f&lt;sub&gt;maxSq&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kΩ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-					 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kHz					 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17-28V </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17-28V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nevyžaduje</t>
   </si>
 </sst>
 </file>
@@ -4354,7 +4454,7 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -4496,6 +4596,467 @@
       <c r="B17" s="1" t="s">
         <v>99</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.23"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
pridan popis DI, DO, AI, CAN a rozpracovane FBE. Popisky jsou klikaci od vsech UNI serv.
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/parameters.xlsx
+++ b/docs/Manual/source/CZ/tab/parameters.xlsx
@@ -32,6 +32,8 @@
     <sheet name="TGMcontroller" sheetId="22" state="visible" r:id="rId24"/>
     <sheet name="TGZpMotion" sheetId="23" state="visible" r:id="rId25"/>
     <sheet name="commonHW_DI" sheetId="24" state="visible" r:id="rId26"/>
+    <sheet name="commonHW_DO" sheetId="25" state="visible" r:id="rId27"/>
+    <sheet name="commonHW_AI" sheetId="26" state="visible" r:id="rId28"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="285">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -768,13 +770,13 @@
     <t xml:space="preserve"> # </t>
   </si>
   <si>
-    <t xml:space="preserve"> U&lt;sub&gt;log0&lt;/sub&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U&lt;sub&gt;log1&lt;/sub&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U&lt;sub&gt;nom&lt;/sub&gt;</t>
+    <t xml:space="preserve"> V&lt;sub&gt;log0&lt;/sub&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V&lt;sub&gt;log1&lt;/sub&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V&lt;sub&gt;nom&lt;/sub&gt;</t>
   </si>
   <si>
     <t xml:space="preserve"> VDD&lt;sub&gt;IO&lt;/sub&gt;</t>
@@ -789,46 +791,141 @@
     <t xml:space="preserve"> I&lt;sub&gt;in28&lt;/sub&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve"> RI&lt;sub&gt;inNom&lt;/sub&gt; </t>
+    <t xml:space="preserve"> R&lt;sub&gt;in,Nom&lt;/sub&gt; </t>
   </si>
   <si>
     <t xml:space="preserve"> Osa č. </t>
   </si>
   <si>
+    <t xml:space="preserve"> f&lt;sub&gt;max,Sq&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kΩ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-					 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kHz					 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17-28V </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17-28V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nevyžaduje</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> č. výstupu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nominální výstupní napětí </t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. napájecí napětí </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. napájecí napětí 𐠒 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">min.výstupní napětí ±20% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. výstupní napětí ±20% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. výstupní proud</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> přiřazeno k ose </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> max. frekvence - obdélník </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VDD&lt;sub&gt;IO,min&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VDD&lt;sub&gt;IO,max&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V&lt;sub&gt;O,min&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V&lt;sub&gt;O,max&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I&lt;sub&gt;O,max&lt;/sub&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve"> f&lt;sub&gt;maxSq&lt;/sub&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> V</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> V </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> kΩ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-					 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kHz					 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0-10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17-28V </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17-28V</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nevyžaduje</t>
+    <t xml:space="preserve"> VDD&lt;sub&gt;IO&lt;/sub&gt; - 0,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rozsah napětí</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nom. vstupní odpor ±10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">časová konstanta ±10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V&lt;sub&gt;in&lt;/sub&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R&lt;sub&gt;inNom&lt;/sub&gt; </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">τ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sub&gt;in&lt;/sub&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">us</t>
   </si>
 </sst>
 </file>
@@ -838,7 +935,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -862,6 +959,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4613,450 +4716,837 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="26.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>239</v>
+      <c r="B1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>250</v>
+      <c r="B2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>257</v>
+      <c r="D3" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>50</v>
+      <c r="C4" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
+      <c r="C5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>